<commit_message>
Added random rngSeed if not specified
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLawIteration.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLawIteration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7646C711-3E4B-45F2-BE37-501D7BCD1DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E1398C-2466-483C-862F-0C516B3D9EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -897,12 +897,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -913,7 +913,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -924,7 +924,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -935,7 +935,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -946,31 +946,28 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="2">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="D26">
-        <v>100</v>
-      </c>
-      <c r="E26">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>104</v>
       </c>
@@ -978,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -989,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>110</v>
       </c>
@@ -997,18 +994,18 @@
         <v>111</v>
       </c>
       <c r="C29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>112</v>
       </c>
       <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>113</v>
       </c>
@@ -1016,21 +1013,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.05</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -1041,7 +1040,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>115</v>
       </c>
@@ -1052,26 +1051,23 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>32</v>
       </c>
       <c r="C37" s="2">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -1082,7 +1078,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -1093,12 +1089,12 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
       <c r="B41" t="s">
         <v>36</v>
@@ -1107,7 +1103,7 @@
         <v>5.9999999999999999E-24</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" t="s">
         <v>121</v>
@@ -1116,12 +1112,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>38</v>
       </c>
@@ -1129,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -1140,12 +1136,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>98</v>
       </c>

</xml_diff>